<commit_message>
update valuetype and alcohol categories
update fruit and veg quantity valuetype and alcohol frequency categories. Also, modify bmi harmo_rule: add a round, 2
</commit_message>
<xml_diff>
--- a/data_processing_elements-AGN.xlsx
+++ b/data_processing_elements-AGN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlaforme\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFA941D-0E2F-4F65-AF8A-F4410B94F258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436E926C-9565-407D-A93F-BA60034CECAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="446">
   <si>
     <t>index</t>
   </si>
@@ -508,9 +508,6 @@
     <t>kg; cm</t>
   </si>
   <si>
-    <t>weight1 / (height1/100)^2</t>
-  </si>
-  <si>
     <t>pm_waist_circ</t>
   </si>
   <si>
@@ -790,11 +787,6 @@
     <t>Fruit Intake frequency</t>
   </si>
   <si>
-    <t>1 = Rarely ; 
-2 = Several times a week ; 
-3 = Every day</t>
-  </si>
-  <si>
     <t>nut_vegetable_quantity</t>
   </si>
   <si>
@@ -838,12 +830,6 @@
   </si>
   <si>
     <t>Frequency of alcohol consumption</t>
-  </si>
-  <si>
-    <t>0 = Never/almost never ; 
-1 = Monthly ; 
-2 = Weekly ; 
-3 = Daily/almost daily</t>
   </si>
   <si>
     <t>smk_smoking_status</t>
@@ -878,11 +864,6 @@
   </si>
   <si>
     <t>Current smoking frequency</t>
-  </si>
-  <si>
-    <t>1 = Monthly ;
-2 = Weekly ;
-3 = Daily/almost daily ;</t>
   </si>
   <si>
     <t>smk_smoking_quantity</t>
@@ -1204,10 +1185,6 @@
     <t>Alzheimers/Dementia</t>
   </si>
   <si>
-    <t>0 = Has not been diagnosed with Alzheimers or other dementia;
-1 = Has been diagnosed with Alzheimers or other dementia</t>
-  </si>
-  <si>
     <t>Category of self-reported physician diagnosed neurologic disease -wave 1</t>
   </si>
   <si>
@@ -1239,17 +1216,6 @@
   </si>
   <si>
     <t>Usual number of hours of sleep - categorical</t>
-  </si>
-  <si>
-    <t>1 = 0 to 6 hours; 
-2 = 6.5 hours;
-3 = 7 hours;
-4 = 7.5 hours;
-5 = 8 hours;
-6 = 8.5 hours;
-7 = 9 hours;
-8 = 9.5 hours;
-9 = 10 hours or more</t>
   </si>
   <si>
     <t>sleep_difficulties</t>
@@ -1353,14 +1319,6 @@
     <t>Overall time spent sitting per day - categorical</t>
   </si>
   <si>
-    <t>0 = None ; 
-1 = Less than 1 hour per day ; 
-2 = One to less than 3 hours per day ; 
-3 = Three to less than 5 hours per day ; 
-4 = Five to less than 7 hours per day ; 
-5 = Seven hours or more per day</t>
-  </si>
-  <si>
     <t>YPAS_sitting1</t>
   </si>
   <si>
@@ -1549,6 +1507,37 @@
   </si>
   <si>
     <t>recode(0=1; 1=1; 2=2; 3=2; 4=3; ELSE=NA)</t>
+  </si>
+  <si>
+    <t>0 = Self-reported ; 
+1 = Measured by professional</t>
+  </si>
+  <si>
+    <t>0 = Rarely ; 
+1 = Several times a week ; 
+2 = Every day</t>
+  </si>
+  <si>
+    <t>0 = Never/almost never ; 
+1 = Monthly; 
+2 = Weekly; 
+3 = Daily/almost daily</t>
+  </si>
+  <si>
+    <t>1 = Occasionaly;
+2 = Daily/almost daily ;</t>
+  </si>
+  <si>
+    <t>0 = Has been diagnosed with Alzheimers or other dementia ; 
+1 = Has not been diagnosed with Alzheimers or other dementia</t>
+  </si>
+  <si>
+    <t>1 = 0 to 6 hours; 
+2 = 7 to 10 hours; 
+3 = 10 hours or more</t>
+  </si>
+  <si>
+    <t>round(weight1 / (height1/100)^2, 2)</t>
   </si>
 </sst>
 </file>
@@ -1651,9 +1640,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1663,13 +1649,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2012,10 +1999,10 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C78" sqref="C78"/>
+      <selection pane="bottomRight" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,6 +2027,7 @@
     <col min="18" max="18" width="17.5703125" style="12" customWidth="1"/>
     <col min="19" max="19" width="19.85546875" style="12" customWidth="1"/>
     <col min="20" max="21" width="9.140625" style="12"/>
+    <col min="22" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -2067,7 +2055,7 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -2079,7 +2067,7 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
@@ -2128,7 +2116,7 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="11"/>
+      <c r="I2" s="9"/>
       <c r="J2" s="1" t="s">
         <v>26</v>
       </c>
@@ -2138,7 +2126,7 @@
       <c r="L2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="9" t="s">
         <v>28</v>
       </c>
       <c r="N2" s="1"/>
@@ -2180,7 +2168,7 @@
       <c r="H3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="11"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="1" t="s">
         <v>37</v>
       </c>
@@ -2190,7 +2178,7 @@
       <c r="L3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="9" t="s">
         <v>40</v>
       </c>
       <c r="N3" s="1"/>
@@ -2230,7 +2218,7 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="9" t="s">
         <v>47</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -2242,7 +2230,7 @@
       <c r="L4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="9" t="s">
         <v>50</v>
       </c>
       <c r="N4" s="1"/>
@@ -2284,7 +2272,7 @@
         <v>56</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="11"/>
+      <c r="I5" s="9"/>
       <c r="J5" s="1" t="s">
         <v>57</v>
       </c>
@@ -2294,7 +2282,7 @@
       <c r="L5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M5" s="11"/>
+      <c r="M5" s="9"/>
       <c r="N5" s="1" t="s">
         <v>56</v>
       </c>
@@ -2309,7 +2297,7 @@
         <v>41</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="U5" s="1"/>
     </row>
@@ -2334,7 +2322,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="9" t="s">
         <v>64</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -2346,7 +2334,7 @@
       <c r="L6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="9" t="s">
         <v>68</v>
       </c>
       <c r="N6" s="1"/>
@@ -2355,7 +2343,7 @@
         <v>82</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>82</v>
@@ -2389,7 +2377,7 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="9" t="s">
         <v>74</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -2397,7 +2385,7 @@
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="11"/>
+      <c r="M7" s="9"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1" t="s">
         <v>76</v>
@@ -2438,7 +2426,7 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="9" t="s">
         <v>81</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -2446,7 +2434,7 @@
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="11"/>
+      <c r="M8" s="9"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
@@ -2484,7 +2472,7 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="9" t="s">
         <v>87</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -2492,7 +2480,7 @@
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="11"/>
+      <c r="M9" s="9"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
         <v>88</v>
@@ -2532,13 +2520,13 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="11"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="11"/>
+      <c r="M10" s="9"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
         <v>88</v>
@@ -2578,13 +2566,13 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="11"/>
+      <c r="I11" s="9"/>
       <c r="J11" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="11"/>
+      <c r="M11" s="9"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
         <v>88</v>
@@ -2624,7 +2612,7 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="9" t="s">
         <v>99</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -2632,7 +2620,7 @@
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="11"/>
+      <c r="M12" s="9"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
@@ -2647,7 +2635,7 @@
       <c r="S12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="T12" s="7" t="s">
+      <c r="T12" s="6" t="s">
         <v>100</v>
       </c>
       <c r="U12" s="1"/>
@@ -2673,7 +2661,7 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="9" t="s">
         <v>104</v>
       </c>
       <c r="J13" s="1" t="s">
@@ -2685,7 +2673,7 @@
       <c r="L13" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="9" t="s">
         <v>108</v>
       </c>
       <c r="N13" s="1"/>
@@ -2725,7 +2713,7 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="9" t="s">
         <v>113</v>
       </c>
       <c r="J14" s="1" t="s">
@@ -2737,7 +2725,7 @@
       <c r="L14" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="M14" s="11" t="s">
+      <c r="M14" s="9" t="s">
         <v>108</v>
       </c>
       <c r="N14" s="1"/>
@@ -2777,7 +2765,7 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="11" t="s">
+      <c r="I15" s="9" t="s">
         <v>117</v>
       </c>
       <c r="J15" s="1" t="s">
@@ -2785,7 +2773,7 @@
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="11"/>
+      <c r="M15" s="9"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1" t="s">
@@ -2828,7 +2816,7 @@
         <v>121</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="11"/>
+      <c r="I16" s="9"/>
       <c r="J16" s="1" t="s">
         <v>122</v>
       </c>
@@ -2838,7 +2826,7 @@
       <c r="L16" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="M16" s="9" t="s">
         <v>40</v>
       </c>
       <c r="N16" s="1" t="s">
@@ -2880,8 +2868,8 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="11" t="s">
-        <v>127</v>
+      <c r="I17" s="9" t="s">
+        <v>439</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>122</v>
@@ -2892,7 +2880,7 @@
       <c r="L17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="M17" s="9" t="s">
         <v>40</v>
       </c>
       <c r="N17" s="1" t="s">
@@ -2936,7 +2924,7 @@
         <v>131</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="11"/>
+      <c r="I18" s="9"/>
       <c r="J18" s="1" t="s">
         <v>132</v>
       </c>
@@ -2946,7 +2934,7 @@
       <c r="L18" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="M18" s="9" t="s">
         <v>40</v>
       </c>
       <c r="N18" s="1" t="s">
@@ -2988,7 +2976,7 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="9" t="s">
         <v>127</v>
       </c>
       <c r="J19" s="1" t="s">
@@ -3000,7 +2988,7 @@
       <c r="L19" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="M19" s="11" t="s">
+      <c r="M19" s="9" t="s">
         <v>40</v>
       </c>
       <c r="N19" s="1" t="s">
@@ -3021,7 +3009,7 @@
       </c>
       <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3044,8 +3032,8 @@
         <v>140</v>
       </c>
       <c r="H20" s="1"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="6" t="s">
+      <c r="I20" s="9"/>
+      <c r="J20" s="1" t="s">
         <v>141</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -3054,7 +3042,7 @@
       <c r="L20" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="M20" s="11" t="s">
+      <c r="M20" s="9" t="s">
         <v>144</v>
       </c>
       <c r="N20" s="1" t="s">
@@ -3071,11 +3059,11 @@
         <v>41</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>146</v>
+        <v>445</v>
       </c>
       <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3083,13 +3071,13 @@
         <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>92</v>
@@ -3098,24 +3086,24 @@
         <v>121</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="6" t="s">
+      <c r="I21" s="9"/>
+      <c r="J21" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="L21" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="M21" s="11" t="s">
+      <c r="N21" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>29</v>
@@ -3127,11 +3115,11 @@
         <v>41</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3139,36 +3127,36 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="J22" s="6" t="s">
+      <c r="I22" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K22" s="6" t="s">
+      <c r="L22" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="M22" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="M22" s="11" t="s">
+      <c r="N22" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1" t="s">
@@ -3181,7 +3169,7 @@
         <v>41</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U22" s="1"/>
     </row>
@@ -3193,36 +3181,36 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="E23" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="M23" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N23" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="M23" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1" t="s">
@@ -3247,34 +3235,34 @@
         <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="11"/>
+      <c r="I24" s="9"/>
       <c r="J24" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="M24" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="M24" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="12" t="s">
@@ -3287,7 +3275,7 @@
         <v>41</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U24" s="1"/>
     </row>
@@ -3299,39 +3287,39 @@
         <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="M25" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="O25" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="M25" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>29</v>
@@ -3355,39 +3343,39 @@
         <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="11"/>
+      <c r="I26" s="9"/>
       <c r="J26" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="L26" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="M26" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="O26" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="M26" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>29</v>
@@ -3411,39 +3399,39 @@
         <v>21</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="M27" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="M27" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="N27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>29</v>
@@ -3467,28 +3455,28 @@
         <v>21</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H28" s="1"/>
-      <c r="I28" s="11"/>
+      <c r="I28" s="9"/>
       <c r="J28" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="11"/>
+      <c r="M28" s="9"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1" t="s">
@@ -3513,28 +3501,28 @@
         <v>21</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="E29" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="11" t="s">
-        <v>194</v>
+      <c r="I29" s="9" t="s">
+        <v>193</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="11"/>
+      <c r="M29" s="9"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1" t="s">
@@ -3559,28 +3547,28 @@
         <v>21</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="E30" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H30" s="1"/>
-      <c r="I30" s="11"/>
+      <c r="I30" s="9"/>
       <c r="J30" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="11"/>
+      <c r="M30" s="9"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1" t="s">
@@ -3605,28 +3593,28 @@
         <v>21</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="E31" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="11"/>
+      <c r="I31" s="9"/>
       <c r="J31" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-      <c r="M31" s="11"/>
+      <c r="M31" s="9"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1" t="s">
@@ -3651,36 +3639,36 @@
         <v>21</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="L32" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="M32" s="11" t="s">
+      <c r="M32" s="9" t="s">
         <v>40</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1" t="s">
@@ -3705,36 +3693,36 @@
         <v>21</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>208</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="11"/>
+      <c r="I33" s="9"/>
       <c r="J33" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="K33" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="L33" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="M33" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="M33" s="9" t="s">
         <v>40</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O33" s="1"/>
       <c r="P33" s="1" t="s">
@@ -3759,36 +3747,36 @@
         <v>21</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>212</v>
-      </c>
       <c r="E34" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="11"/>
+      <c r="I34" s="9"/>
       <c r="J34" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="K34" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="L34" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="M34" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="M34" s="9" t="s">
         <v>40</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1" t="s">
@@ -3813,28 +3801,28 @@
         <v>21</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="E35" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="11"/>
+      <c r="I35" s="9"/>
       <c r="J35" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-      <c r="M35" s="11"/>
+      <c r="M35" s="9"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1" t="s">
@@ -3859,28 +3847,28 @@
         <v>21</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="E36" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H36" s="1"/>
-      <c r="I36" s="11"/>
+      <c r="I36" s="9"/>
       <c r="J36" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
-      <c r="M36" s="11"/>
+      <c r="M36" s="9"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1" t="s">
@@ -3905,36 +3893,36 @@
         <v>21</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="E37" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="L37" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="M37" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="L37" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="M37" s="11" t="s">
+      <c r="N37" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1" t="s">
@@ -3959,33 +3947,33 @@
         <v>21</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="1"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="H38" s="1"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="M38" s="9" t="s">
         <v>232</v>
-      </c>
-      <c r="M38" s="11" t="s">
-        <v>233</v>
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -3993,7 +3981,7 @@
         <v>82</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R38" s="1" t="s">
         <v>82</v>
@@ -4011,33 +3999,33 @@
         <v>21</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="11" t="s">
-        <v>238</v>
+      <c r="I39" s="9" t="s">
+        <v>440</v>
       </c>
       <c r="J39" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K39" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="M39" s="9" t="s">
         <v>232</v>
-      </c>
-      <c r="M39" s="11" t="s">
-        <v>233</v>
       </c>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
@@ -4045,7 +4033,7 @@
         <v>82</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R39" s="1" t="s">
         <v>82</v>
@@ -4063,33 +4051,33 @@
         <v>21</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="F40" s="1" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="G40" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="H40" s="1"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="L40" s="1" t="s">
+      <c r="M40" s="9" t="s">
         <v>232</v>
-      </c>
-      <c r="M40" s="11" t="s">
-        <v>233</v>
       </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
@@ -4097,7 +4085,7 @@
         <v>82</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R40" s="1" t="s">
         <v>82</v>
@@ -4115,33 +4103,33 @@
         <v>21</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="11" t="s">
-        <v>238</v>
+      <c r="I41" s="9" t="s">
+        <v>440</v>
       </c>
       <c r="J41" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K41" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="L41" s="1" t="s">
+      <c r="M41" s="9" t="s">
         <v>232</v>
-      </c>
-      <c r="M41" s="11" t="s">
-        <v>233</v>
       </c>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
@@ -4149,7 +4137,7 @@
         <v>82</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R41" s="1" t="s">
         <v>82</v>
@@ -4167,28 +4155,28 @@
         <v>21</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="11"/>
+      <c r="I42" s="9"/>
       <c r="J42" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="11"/>
+      <c r="M42" s="9"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1" t="s">
@@ -4213,35 +4201,35 @@
         <v>21</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="11"/>
+      <c r="I43" s="9"/>
       <c r="J43" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
-      <c r="M43" s="11"/>
+      <c r="M43" s="9"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1" t="s">
         <v>82</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R43" s="1" t="s">
         <v>82</v>
@@ -4259,35 +4247,35 @@
         <v>21</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="11" t="s">
-        <v>254</v>
+      <c r="I44" s="9" t="s">
+        <v>441</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-      <c r="M44" s="11"/>
+      <c r="M44" s="9"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1" t="s">
         <v>82</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R44" s="1" t="s">
         <v>82</v>
@@ -4305,33 +4293,33 @@
         <v>21</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-      <c r="I45" s="11" t="s">
+      <c r="I45" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="L45" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="M45" s="9" t="s">
         <v>259</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="M45" s="11" t="s">
-        <v>262</v>
       </c>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
@@ -4357,33 +4345,33 @@
         <v>21</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="11" t="s">
-        <v>265</v>
+      <c r="I46" s="9" t="s">
+        <v>442</v>
       </c>
       <c r="J46" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="M46" s="9" t="s">
         <v>259</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="M46" s="11" t="s">
-        <v>262</v>
       </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
@@ -4397,7 +4385,7 @@
         <v>51</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="U46" s="1"/>
     </row>
@@ -4409,28 +4397,28 @@
         <v>21</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="H47" s="1"/>
-      <c r="I47" s="11"/>
+      <c r="I47" s="9"/>
       <c r="J47" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-      <c r="M47" s="11"/>
+      <c r="M47" s="9"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1" t="s">
@@ -4455,33 +4443,33 @@
         <v>21</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-      <c r="I48" s="11" t="s">
+      <c r="I48" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="M48" s="9" t="s">
         <v>271</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="M48" s="11" t="s">
-        <v>275</v>
       </c>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -4495,11 +4483,11 @@
         <v>51</v>
       </c>
       <c r="S48" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="U48" s="1"/>
     </row>
-    <row r="49" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -4507,37 +4495,37 @@
         <v>21</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
-      <c r="I49" s="11" t="s">
+      <c r="I49" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="M49" s="9" t="s">
         <v>280</v>
-      </c>
-      <c r="J49" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="K49" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="M49" s="11" t="s">
-        <v>284</v>
       </c>
       <c r="N49" s="1"/>
       <c r="O49" s="1" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="P49" s="1" t="s">
         <v>29</v>
@@ -4546,17 +4534,17 @@
         <v>69</v>
       </c>
       <c r="R49" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="S49" s="6" t="s">
-        <v>436</v>
-      </c>
-      <c r="T49" s="7" t="s">
-        <v>285</v>
+        <v>312</v>
+      </c>
+      <c r="S49" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="T49" s="6" t="s">
+        <v>281</v>
       </c>
       <c r="U49" s="1"/>
     </row>
-    <row r="50" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -4564,36 +4552,36 @@
         <v>21</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
-      <c r="I50" s="11" t="s">
-        <v>280</v>
+      <c r="I50" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="M50" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="M50" s="9" t="s">
         <v>40</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="P50" s="1" t="s">
         <v>29</v>
@@ -4602,13 +4590,13 @@
         <v>69</v>
       </c>
       <c r="R50" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="S50" s="6" t="s">
-        <v>438</v>
-      </c>
-      <c r="T50" s="7" t="s">
-        <v>292</v>
+        <v>312</v>
+      </c>
+      <c r="S50" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="T50" s="6" t="s">
+        <v>288</v>
       </c>
       <c r="U50" s="1"/>
     </row>
@@ -4620,33 +4608,33 @@
         <v>21</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="11" t="s">
-        <v>280</v>
+      <c r="I51" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="M51" s="11" t="s">
-        <v>298</v>
+        <v>293</v>
+      </c>
+      <c r="M51" s="9" t="s">
+        <v>294</v>
       </c>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
@@ -4660,7 +4648,7 @@
         <v>51</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="U51" s="1"/>
     </row>
@@ -4672,33 +4660,33 @@
         <v>21</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
-      <c r="I52" s="11" t="s">
-        <v>302</v>
+      <c r="I52" s="9" t="s">
+        <v>298</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="L52" s="1"/>
-      <c r="M52" s="11"/>
+      <c r="M52" s="9"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="P52" s="1" t="s">
         <v>29</v>
@@ -4712,8 +4700,8 @@
       <c r="S52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="T52" s="7" t="s">
-        <v>303</v>
+      <c r="T52" s="6" t="s">
+        <v>299</v>
       </c>
       <c r="U52" s="1"/>
     </row>
@@ -4725,33 +4713,33 @@
         <v>21</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
-      <c r="I53" s="11" t="s">
-        <v>280</v>
+      <c r="I53" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="M53" s="11" t="s">
-        <v>298</v>
+        <v>303</v>
+      </c>
+      <c r="M53" s="9" t="s">
+        <v>294</v>
       </c>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
@@ -4765,7 +4753,7 @@
         <v>51</v>
       </c>
       <c r="S53" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="U53" s="1"/>
     </row>
@@ -4777,28 +4765,28 @@
         <v>21</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
-      <c r="I54" s="11" t="s">
-        <v>280</v>
+      <c r="I54" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
-      <c r="M54" s="11"/>
+      <c r="M54" s="9"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1" t="s">
@@ -4815,7 +4803,7 @@
       </c>
       <c r="U54" s="1"/>
     </row>
-    <row r="55" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -4823,32 +4811,32 @@
         <v>21</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
-      <c r="I55" s="11" t="s">
-        <v>280</v>
+      <c r="I55" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="M55" s="11"/>
+        <v>311</v>
+      </c>
+      <c r="M55" s="9"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
       <c r="P55" s="1" t="s">
@@ -4858,14 +4846,14 @@
         <v>69</v>
       </c>
       <c r="R55" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="S55" s="6" t="s">
-        <v>317</v>
+        <v>312</v>
+      </c>
+      <c r="S55" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="U55" s="1"/>
     </row>
-    <row r="56" spans="1:21" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -4873,32 +4861,32 @@
         <v>21</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
-      <c r="I56" s="11" t="s">
-        <v>280</v>
+      <c r="I56" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="M56" s="11"/>
+        <v>311</v>
+      </c>
+      <c r="M56" s="9"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1" t="s">
@@ -4908,17 +4896,17 @@
         <v>69</v>
       </c>
       <c r="R56" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="S56" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="S56" s="6" t="s">
-        <v>320</v>
-      </c>
       <c r="T56" s="13" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="U56" s="1"/>
     </row>
-    <row r="57" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -4926,32 +4914,32 @@
         <v>21</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
-      <c r="I57" s="11" t="s">
-        <v>280</v>
+      <c r="I57" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="M57" s="11"/>
+        <v>311</v>
+      </c>
+      <c r="M57" s="9"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1" t="s">
@@ -4961,10 +4949,10 @@
         <v>69</v>
       </c>
       <c r="R57" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="S57" s="6" t="s">
-        <v>324</v>
+        <v>312</v>
+      </c>
+      <c r="S57" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="U57" s="1"/>
     </row>
@@ -4976,33 +4964,33 @@
         <v>21</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
-      <c r="I58" s="11" t="s">
-        <v>280</v>
+      <c r="I58" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="M58" s="11" t="s">
-        <v>298</v>
+        <v>326</v>
+      </c>
+      <c r="M58" s="9" t="s">
+        <v>294</v>
       </c>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
@@ -5028,31 +5016,31 @@
         <v>21</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
-      <c r="I59" s="11"/>
+      <c r="I59" s="9"/>
       <c r="J59" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="M59" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
+      </c>
+      <c r="M59" s="9" t="s">
+        <v>332</v>
       </c>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
@@ -5078,26 +5066,26 @@
         <v>21</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
-      <c r="I60" s="11"/>
+      <c r="I60" s="9"/>
       <c r="J60" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
-      <c r="M60" s="11"/>
+      <c r="M60" s="9"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
       <c r="P60" s="1" t="s">
@@ -5122,26 +5110,26 @@
         <v>21</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="11"/>
+      <c r="I61" s="9"/>
       <c r="J61" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
-      <c r="M61" s="11"/>
+      <c r="M61" s="9"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
       <c r="P61" s="1" t="s">
@@ -5166,26 +5154,26 @@
         <v>21</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
-      <c r="I62" s="11"/>
+      <c r="I62" s="9"/>
       <c r="J62" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
-      <c r="M62" s="11"/>
+      <c r="M62" s="9"/>
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
       <c r="P62" s="1" t="s">
@@ -5210,26 +5198,26 @@
         <v>21</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
-      <c r="I63" s="11"/>
+      <c r="I63" s="9"/>
       <c r="J63" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
-      <c r="M63" s="11"/>
+      <c r="M63" s="9"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
       <c r="P63" s="1" t="s">
@@ -5254,30 +5242,30 @@
         <v>21</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
-      <c r="I64" s="11"/>
+      <c r="I64" s="9"/>
       <c r="J64" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="M64" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="M64" s="9" t="s">
         <v>40</v>
       </c>
       <c r="N64" s="1"/>
@@ -5304,26 +5292,26 @@
         <v>21</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
-      <c r="I65" s="11"/>
+      <c r="I65" s="9"/>
       <c r="J65" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
-      <c r="M65" s="11"/>
+      <c r="M65" s="9"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
       <c r="P65" s="1" t="s">
@@ -5340,7 +5328,7 @@
       </c>
       <c r="U65" s="1"/>
     </row>
-    <row r="66" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -5348,33 +5336,33 @@
         <v>21</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
-      <c r="I66" s="11" t="s">
-        <v>354</v>
-      </c>
-      <c r="J66" s="6" t="s">
-        <v>441</v>
+      <c r="I66" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>434</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="M66" s="11" t="s">
-        <v>357</v>
+        <v>351</v>
+      </c>
+      <c r="M66" s="9" t="s">
+        <v>352</v>
       </c>
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
@@ -5385,13 +5373,13 @@
         <v>69</v>
       </c>
       <c r="R66" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="S66" s="6" t="s">
-        <v>443</v>
-      </c>
-      <c r="T66" s="7" t="s">
-        <v>358</v>
+        <v>312</v>
+      </c>
+      <c r="S66" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="T66" s="6" t="s">
+        <v>353</v>
       </c>
       <c r="U66" s="1"/>
     </row>
@@ -5403,28 +5391,28 @@
         <v>21</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="H67" s="1"/>
-      <c r="I67" s="11"/>
+      <c r="I67" s="9"/>
       <c r="J67" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
-      <c r="M67" s="11"/>
+      <c r="M67" s="9"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
       <c r="P67" s="1" t="s">
@@ -5449,28 +5437,28 @@
         <v>21</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
-      <c r="I68" s="11" t="s">
-        <v>364</v>
+      <c r="I68" s="9" t="s">
+        <v>444</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
-      <c r="M68" s="11"/>
+      <c r="M68" s="9"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
       <c r="P68" s="1" t="s">
@@ -5495,28 +5483,28 @@
         <v>21</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
-      <c r="I69" s="11" t="s">
-        <v>367</v>
+      <c r="I69" s="9" t="s">
+        <v>361</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
-      <c r="M69" s="11"/>
+      <c r="M69" s="9"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
       <c r="P69" s="1" t="s">
@@ -5541,28 +5529,28 @@
         <v>21</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
-      <c r="I70" s="11" t="s">
-        <v>370</v>
+      <c r="I70" s="9" t="s">
+        <v>364</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
-      <c r="M70" s="11"/>
+      <c r="M70" s="9"/>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
       <c r="P70" s="1" t="s">
@@ -5587,28 +5575,28 @@
         <v>21</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
-      <c r="I71" s="11" t="s">
-        <v>370</v>
+      <c r="I71" s="9" t="s">
+        <v>364</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
-      <c r="M71" s="11"/>
+      <c r="M71" s="9"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
       <c r="P71" s="1" t="s">
@@ -5633,28 +5621,28 @@
         <v>21</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
-      <c r="I72" s="11" t="s">
-        <v>370</v>
+      <c r="I72" s="9" t="s">
+        <v>364</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
-      <c r="M72" s="11"/>
+      <c r="M72" s="9"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
       <c r="P72" s="1" t="s">
@@ -5679,28 +5667,28 @@
         <v>21</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
-      <c r="I73" s="11" t="s">
-        <v>378</v>
+      <c r="I73" s="9" t="s">
+        <v>372</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
-      <c r="M73" s="11"/>
+      <c r="M73" s="9"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
       <c r="P73" s="1" t="s">
@@ -5725,28 +5713,28 @@
         <v>21</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
-      <c r="I74" s="11" t="s">
-        <v>382</v>
+      <c r="I74" s="9" t="s">
+        <v>376</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
-      <c r="M74" s="11"/>
+      <c r="M74" s="9"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
       <c r="P74" s="1" t="s">
@@ -5771,28 +5759,28 @@
         <v>21</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
-      <c r="I75" s="11" t="s">
-        <v>386</v>
+      <c r="I75" s="9" t="s">
+        <v>380</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
-      <c r="M75" s="11"/>
+      <c r="M75" s="9"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
       <c r="P75" s="1" t="s">
@@ -5817,28 +5805,28 @@
         <v>21</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="H76" s="1"/>
-      <c r="I76" s="11"/>
+      <c r="I76" s="9"/>
       <c r="J76" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
-      <c r="M76" s="11"/>
+      <c r="M76" s="9"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
       <c r="P76" s="1" t="s">
@@ -5863,34 +5851,29 @@
         <v>21</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="F77" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G77" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="I77" s="14" t="s">
-        <v>393</v>
-      </c>
+      <c r="G77" s="1"/>
       <c r="J77" s="1" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="M77" s="11" t="s">
-        <v>397</v>
+        <v>389</v>
+      </c>
+      <c r="M77" s="9" t="s">
+        <v>390</v>
       </c>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
@@ -5904,7 +5887,7 @@
         <v>51</v>
       </c>
       <c r="S77" s="1" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="U77" s="1"/>
     </row>
@@ -5916,37 +5899,37 @@
         <v>21</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
-      <c r="I78" s="11" t="s">
-        <v>402</v>
+      <c r="I78" s="9" t="s">
+        <v>395</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="M78" s="11" t="s">
-        <v>406</v>
+        <v>398</v>
+      </c>
+      <c r="M78" s="9" t="s">
+        <v>399</v>
       </c>
       <c r="N78" s="1"/>
       <c r="O78" s="1" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="P78" s="1" t="s">
         <v>29</v>
@@ -5958,7 +5941,7 @@
         <v>51</v>
       </c>
       <c r="S78" s="1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="U78" s="1"/>
     </row>
@@ -5970,28 +5953,28 @@
         <v>21</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
-      <c r="I79" s="11" t="s">
-        <v>410</v>
+      <c r="I79" s="9" t="s">
+        <v>403</v>
       </c>
       <c r="J79" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
-      <c r="M79" s="11"/>
+      <c r="M79" s="9"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
       <c r="P79" s="1" t="s">
@@ -6016,33 +5999,33 @@
         <v>21</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
-      <c r="I80" s="11" t="s">
-        <v>280</v>
+      <c r="I80" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="M80" s="11" t="s">
-        <v>417</v>
+        <v>409</v>
+      </c>
+      <c r="M80" s="9" t="s">
+        <v>410</v>
       </c>
       <c r="N80" s="1"/>
       <c r="P80" s="1" t="s">
@@ -6055,7 +6038,7 @@
         <v>51</v>
       </c>
       <c r="S80" s="1" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="U80" s="1"/>
     </row>
@@ -6067,28 +6050,28 @@
         <v>21</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
-      <c r="I81" s="11" t="s">
-        <v>280</v>
+      <c r="I81" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
-      <c r="M81" s="11"/>
+      <c r="M81" s="9"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
       <c r="P81" s="1" t="s">
@@ -6113,33 +6096,33 @@
         <v>21</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
-      <c r="I82" s="11" t="s">
-        <v>280</v>
+      <c r="I82" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="L82" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="M82" s="11" t="s">
-        <v>417</v>
+        <v>409</v>
+      </c>
+      <c r="M82" s="9" t="s">
+        <v>410</v>
       </c>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
@@ -6153,7 +6136,7 @@
         <v>51</v>
       </c>
       <c r="S82" s="1" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="U82" s="1"/>
     </row>
@@ -6165,26 +6148,26 @@
         <v>21</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
-      <c r="I83" s="11"/>
+      <c r="I83" s="9"/>
       <c r="J83" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
-      <c r="M83" s="11"/>
+      <c r="M83" s="9"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
       <c r="P83" s="1" t="s">
@@ -6209,28 +6192,28 @@
         <v>21</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="H84" s="1"/>
-      <c r="I84" s="11"/>
+      <c r="I84" s="9"/>
       <c r="J84" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
-      <c r="M84" s="11"/>
+      <c r="M84" s="9"/>
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
       <c r="P84" s="1" t="s">

</xml_diff>